<commit_message>
added screnshots folder, added explicit and implicit wait to Utility package
</commit_message>
<xml_diff>
--- a/src/Data/LogIn.xlsx
+++ b/src/Data/LogIn.xlsx
@@ -3,14 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_projects\AutomationPractice\AutomationPracticeTest\src\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="3330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>test ID</t>
   </si>
@@ -88,7 +92,7 @@
     <t>8L</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>fdklh@kkdsg.com</t>
   </si>
   <si>
     <t>9L</t>
@@ -127,10 +131,13 @@
     <t>hdfjhgjk</t>
   </si>
   <si>
+    <t>create-email</t>
+  </si>
+  <si>
+    <t>An account using this email address has already been registered. Please enter a valid password or request a new one.</t>
+  </si>
+  <si>
     <t>signIn-email</t>
-  </si>
-  <si>
-    <t>create-email</t>
   </si>
 </sst>
 </file>
@@ -226,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,6 +244,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,11 +256,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,14 +551,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -569,7 +585,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -582,7 +598,7 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -591,11 +607,11 @@
         <v>7</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -610,7 +626,7 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -625,7 +641,7 @@
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -640,7 +656,7 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -649,29 +665,27 @@
         <v>18</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
+      <c r="C9" s="9"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -679,13 +693,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -693,12 +707,12 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="3" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -706,12 +720,12 @@
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -719,12 +733,12 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -732,12 +746,12 @@
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -745,12 +759,12 @@
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -758,9 +772,9 @@
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1"/>
     <hyperlink ref="C8" r:id="rId2"/>
-    <hyperlink ref="C9" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-    <hyperlink ref="B14" r:id="rId5"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>